<commit_message>
Published state of ETDataset on 19 September 2014.
</commit_message>
<xml_diff>
--- a/analyses/7_services_analysis.xlsx
+++ b/analyses/7_services_analysis.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15400" tabRatio="929" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15960" tabRatio="929" firstSheet="15" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="34" r:id="rId1"/>
@@ -1484,12 +1484,6 @@
     <t>buildings_space_heater_heatpump_air_water_network_gas</t>
   </si>
   <si>
-    <t>buildings_final_demand_for_space_heating_gas</t>
-  </si>
-  <si>
-    <t>buildings_final_demand_for_space_heating_gas_parent_share</t>
-  </si>
-  <si>
     <t>buildings_final_demand_coal_parent_share</t>
   </si>
   <si>
@@ -1500,12 +1494,6 @@
   </si>
   <si>
     <t>buildings_final_demand_network_gas_parent_share</t>
-  </si>
-  <si>
-    <t>buildings_final_demand_for_appliances_gas</t>
-  </si>
-  <si>
-    <t>buildings_final_demand_for_cooling_gas</t>
   </si>
   <si>
     <t>buildings_final_demand_crude_oil_parent_share</t>
@@ -2151,6 +2139,18 @@
   </si>
   <si>
     <t>Implemented if-statement in Technology share to avoid #DIV/0 errors</t>
+  </si>
+  <si>
+    <t>buildings_final_demand_for_space_heating_network_gas</t>
+  </si>
+  <si>
+    <t>buildings_final_demand_for_cooling_network_gas</t>
+  </si>
+  <si>
+    <t>buildings_final_demand_for_appliances_network_gas</t>
+  </si>
+  <si>
+    <t>buildings_final_demand_for_space_heating_network_gas_parent_share</t>
   </si>
 </sst>
 </file>
@@ -9567,7 +9567,7 @@
   <dimension ref="B2:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9603,13 +9603,13 @@
     <row r="6" spans="2:5" ht="16" thickBot="1"/>
     <row r="7" spans="2:5" ht="30">
       <c r="B7" s="201" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="C7" s="283" t="s">
         <v>341</v>
       </c>
       <c r="D7" s="167" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="E7" s="168" t="s">
         <v>346</v>
@@ -9659,7 +9659,7 @@
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="279" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="C12" s="169"/>
       <c r="D12" s="223"/>
@@ -9888,10 +9888,10 @@
     <row r="6" spans="2:6" ht="16" thickBot="1"/>
     <row r="7" spans="2:6" ht="30">
       <c r="B7" s="201" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="C7" s="274" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="D7" s="283" t="s">
         <v>229</v>
@@ -9900,7 +9900,7 @@
         <v>351</v>
       </c>
       <c r="F7" s="168" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
     </row>
     <row r="8" spans="2:6">
@@ -9915,7 +9915,7 @@
     <row r="9" spans="2:6">
       <c r="B9" s="280"/>
       <c r="C9" s="60" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>123</v>
@@ -9954,7 +9954,7 @@
     <row r="12" spans="2:6">
       <c r="B12" s="280"/>
       <c r="C12" s="60" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>125</v>
@@ -10002,7 +10002,7 @@
     <row r="16" spans="2:6">
       <c r="B16" s="280"/>
       <c r="C16" s="60" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>125</v>
@@ -10050,7 +10050,7 @@
     <row r="20" spans="2:6">
       <c r="B20" s="280"/>
       <c r="C20" s="60" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>134</v>
@@ -10205,7 +10205,7 @@
     </row>
     <row r="5" spans="1:11" ht="30" customHeight="1">
       <c r="B5" s="400" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="C5" s="402"/>
       <c r="D5" s="402"/>
@@ -10263,28 +10263,28 @@
         <v>132</v>
       </c>
       <c r="D9" s="108" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="E9" s="69" t="s">
+        <v>484</v>
+      </c>
+      <c r="F9" s="69" t="s">
+        <v>602</v>
+      </c>
+      <c r="G9" s="69" t="s">
+        <v>485</v>
+      </c>
+      <c r="H9" s="69" t="s">
+        <v>486</v>
+      </c>
+      <c r="I9" s="69" t="s">
+        <v>487</v>
+      </c>
+      <c r="J9" s="69" t="s">
         <v>488</v>
       </c>
-      <c r="F9" s="69" t="s">
-        <v>606</v>
-      </c>
-      <c r="G9" s="69" t="s">
+      <c r="K9" s="146" t="s">
         <v>489</v>
-      </c>
-      <c r="H9" s="69" t="s">
-        <v>490</v>
-      </c>
-      <c r="I9" s="69" t="s">
-        <v>491</v>
-      </c>
-      <c r="J9" s="69" t="s">
-        <v>492</v>
-      </c>
-      <c r="K9" s="146" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -10804,7 +10804,7 @@
     <row r="38" spans="2:12">
       <c r="B38" s="30"/>
       <c r="C38" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="D38" s="75"/>
       <c r="E38" s="257" t="e">
@@ -10851,7 +10851,7 @@
     </row>
     <row r="40" spans="2:12">
       <c r="B40" s="396" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="5"/>
@@ -10883,7 +10883,7 @@
     <row r="42" spans="2:12">
       <c r="B42" s="30"/>
       <c r="C42" s="17" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="D42" s="75"/>
       <c r="E42" s="257" t="e">
@@ -10899,16 +10899,16 @@
         <v>#DIV/0!</v>
       </c>
       <c r="H42" s="383" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="I42" s="383" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="J42" s="383" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="K42" s="391" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="43" spans="2:12" ht="16" thickBot="1">
@@ -10995,7 +10995,7 @@
     <row r="6" spans="2:10" ht="16" thickBot="1"/>
     <row r="7" spans="2:10">
       <c r="B7" s="27" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="C7" s="53"/>
       <c r="D7" s="28"/>
@@ -11757,7 +11757,7 @@
         <v>274</v>
       </c>
       <c r="D9" s="69" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="E9" s="69" t="s">
         <v>275</v>
@@ -11778,10 +11778,10 @@
         <v>290</v>
       </c>
       <c r="K9" s="265" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="L9" s="146" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
     </row>
     <row r="10" spans="2:13">
@@ -11869,13 +11869,13 @@
     </row>
     <row r="17" spans="10:11">
       <c r="J17" s="259" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="K17" s="203"/>
     </row>
     <row r="18" spans="10:11">
       <c r="J18" s="260" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="K18" s="261"/>
     </row>
@@ -11895,13 +11895,13 @@
     </row>
     <row r="21" spans="10:11">
       <c r="J21" s="260" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="K21" s="261"/>
     </row>
     <row r="22" spans="10:11">
       <c r="J22" s="260" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="K22" s="261"/>
     </row>
@@ -11911,7 +11911,7 @@
     </row>
     <row r="24" spans="10:11">
       <c r="J24" s="262" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="K24" s="263">
         <f>K11-Final_demand_residences</f>
@@ -12021,10 +12021,10 @@
         <v>301</v>
       </c>
       <c r="E8" s="108" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="F8" s="108" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="G8" s="190" t="s">
         <v>302</v>
@@ -12771,7 +12771,7 @@
         <v>41485</v>
       </c>
       <c r="C23" s="39" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D23" s="309">
         <v>1.18</v>
@@ -12783,7 +12783,7 @@
         <v>41485</v>
       </c>
       <c r="C24" s="39" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="D24" s="309">
         <v>1.18</v>
@@ -12795,7 +12795,7 @@
         <v>41486</v>
       </c>
       <c r="C25" s="39" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="D25" s="309">
         <v>1.19</v>
@@ -12807,7 +12807,7 @@
         <v>41487</v>
       </c>
       <c r="C26" s="39" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D26" s="309">
         <v>1.19</v>
@@ -12819,7 +12819,7 @@
         <v>41499</v>
       </c>
       <c r="C27" s="39" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="D27" s="308">
         <v>1.2</v>
@@ -12831,7 +12831,7 @@
         <v>41500</v>
       </c>
       <c r="C28" s="39" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="D28" s="309">
         <v>1.21</v>
@@ -12843,7 +12843,7 @@
         <v>41500</v>
       </c>
       <c r="C29" s="39" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="D29" s="308">
         <v>1.22</v>
@@ -12855,7 +12855,7 @@
         <v>41502</v>
       </c>
       <c r="C30" s="39" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="D30" s="308">
         <v>1.23</v>
@@ -12867,7 +12867,7 @@
         <v>41505</v>
       </c>
       <c r="C31" s="39" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="D31" s="308">
         <v>1.24</v>
@@ -12879,7 +12879,7 @@
         <v>41506</v>
       </c>
       <c r="C32" s="39" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="D32" s="308">
         <v>1.25</v>
@@ -12891,7 +12891,7 @@
         <v>41507</v>
       </c>
       <c r="C33" s="39" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="D33" s="308">
         <v>1.26</v>
@@ -12903,7 +12903,7 @@
         <v>41509</v>
       </c>
       <c r="C34" s="39" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="D34" s="308">
         <v>1.27</v>
@@ -12915,7 +12915,7 @@
         <v>41509</v>
       </c>
       <c r="C35" s="39" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="D35" s="308">
         <v>1.28</v>
@@ -12924,10 +12924,10 @@
     </row>
     <row r="36" spans="2:5">
       <c r="B36" s="305" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="C36" s="39" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D36" s="308">
         <v>1.29</v>
@@ -12939,7 +12939,7 @@
         <v>41534</v>
       </c>
       <c r="C37" s="39" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="D37" s="308">
         <v>1.3</v>
@@ -12951,7 +12951,7 @@
         <v>41542</v>
       </c>
       <c r="C38" s="39" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="D38" s="308">
         <v>1.31</v>
@@ -12963,7 +12963,7 @@
         <v>41562</v>
       </c>
       <c r="C39" s="371" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="D39" s="308">
         <v>1.32</v>
@@ -12975,7 +12975,7 @@
         <v>41578</v>
       </c>
       <c r="C40" s="39" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="D40" s="308">
         <v>1.33</v>
@@ -12987,7 +12987,7 @@
         <v>41578</v>
       </c>
       <c r="C41" s="39" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="D41" s="308">
         <v>1.34</v>
@@ -12999,7 +12999,7 @@
         <v>41782</v>
       </c>
       <c r="C42" s="39" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="D42" s="308">
         <v>1.35</v>
@@ -13011,7 +13011,7 @@
         <v>41782</v>
       </c>
       <c r="C43" s="39" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="D43" s="308">
         <v>1.36</v>
@@ -13070,9 +13070,7 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -13081,7 +13079,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="205" t="s">
-        <v>392</v>
+        <v>610</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -13148,7 +13146,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="205" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -13161,7 +13159,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="205" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B3" s="284" t="e">
         <f>'Application shares'!E9</f>
@@ -13170,7 +13168,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="205" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B4" s="284" t="e">
         <f>'Application shares'!E10</f>
@@ -13205,17 +13203,17 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="205" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -13228,7 +13226,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="205" t="s">
-        <v>391</v>
+        <v>607</v>
       </c>
       <c r="B3" s="284" t="e">
         <f>'Application shares'!E13</f>
@@ -13237,7 +13235,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="205" t="s">
-        <v>398</v>
+        <v>608</v>
       </c>
       <c r="B4" s="284" t="e">
         <f>'Application shares'!E14</f>
@@ -13246,7 +13244,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="205" t="s">
-        <v>397</v>
+        <v>609</v>
       </c>
       <c r="B5" s="284" t="e">
         <f>'Application shares'!E15</f>
@@ -13288,7 +13286,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="205" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -13301,7 +13299,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="205" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="B3" s="284" t="e">
         <f>'Application shares'!E18</f>
@@ -13310,7 +13308,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="205" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="B4" s="284" t="e">
         <f>'Application shares'!E19</f>
@@ -13355,7 +13353,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="205" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -13395,7 +13393,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="205" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="B6" s="284" t="e">
         <f>'Application shares'!E25</f>
@@ -13434,7 +13432,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="205" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -13447,7 +13445,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="205" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="B3" s="284">
         <f>Dashboard!E62</f>
@@ -13456,7 +13454,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="205" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="B4" s="284">
         <f>Dashboard!E63</f>
@@ -13502,7 +13500,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -13515,7 +13513,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="B3" s="284">
         <v>0</v>
@@ -13523,7 +13521,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="B4" s="284">
         <v>1</v>
@@ -13568,7 +13566,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -13581,7 +13579,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B3" s="284">
         <v>0</v>
@@ -13589,7 +13587,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="B4" s="284">
         <v>1</v>
@@ -13634,7 +13632,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -13647,7 +13645,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B3" s="284">
         <f>1-B4</f>
@@ -13656,7 +13654,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="B4" s="284">
         <f>Dashboard!E65</f>
@@ -13702,7 +13700,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -13715,7 +13713,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="B3" s="284">
         <f>1-B4</f>
@@ -13724,7 +13722,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B4" s="284">
         <f>Dashboard!E66</f>
@@ -13845,7 +13843,7 @@
     </row>
     <row r="13" spans="2:3" ht="28" customHeight="1">
       <c r="B13" s="177" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="C13" s="61" t="s">
         <v>321</v>
@@ -13861,7 +13859,7 @@
     </row>
     <row r="15" spans="2:3" ht="28" customHeight="1">
       <c r="B15" s="300" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="C15" s="61" t="s">
         <v>347</v>
@@ -13869,7 +13867,7 @@
     </row>
     <row r="16" spans="2:3" ht="28" customHeight="1">
       <c r="B16" s="300" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="C16" s="61" t="s">
         <v>345</v>
@@ -13885,7 +13883,7 @@
     </row>
     <row r="18" spans="2:3" ht="28" customHeight="1">
       <c r="B18" s="126" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="C18" s="61" t="s">
         <v>319</v>
@@ -13896,7 +13894,7 @@
         <v>317</v>
       </c>
       <c r="C19" s="61" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="28" customHeight="1">
@@ -13917,106 +13915,106 @@
     </row>
     <row r="22" spans="2:3" ht="28" customHeight="1">
       <c r="B22" s="178" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C22" s="256" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="28" customHeight="1">
       <c r="B23" s="178" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="C23" s="256" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="24" spans="2:3" ht="28" customHeight="1">
       <c r="B24" s="178" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="C24" s="256" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="28" customHeight="1">
       <c r="B25" s="178" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="C25" s="256" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="26" spans="2:3" ht="28" customHeight="1">
       <c r="B26" s="178" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="C26" s="256" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="27" spans="2:3" ht="28" customHeight="1">
       <c r="B27" s="178" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="C27" s="256" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="28" spans="2:3" ht="28" customHeight="1">
       <c r="B28" s="178" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="C28" s="256" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="29" spans="2:3" ht="28" customHeight="1">
       <c r="B29" s="178" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="C29" s="256" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="30" spans="2:3" ht="28" customHeight="1">
       <c r="B30" s="178" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="C30" s="256" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
     </row>
     <row r="31" spans="2:3" ht="28" customHeight="1">
       <c r="B31" s="178" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="C31" s="256" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
     </row>
     <row r="32" spans="2:3" ht="28" customHeight="1">
       <c r="B32" s="178" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="C32" s="256" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
     </row>
     <row r="33" spans="2:3" ht="28" customHeight="1">
       <c r="B33" s="178" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="C33" s="256" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="28" customHeight="1">
       <c r="B34" s="178" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="C34" s="256" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
     </row>
     <row r="35" spans="2:3" ht="28" customHeight="1"/>
@@ -14063,7 +14061,7 @@
     </row>
     <row r="6" spans="2:2" ht="75">
       <c r="B6" s="113" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
     </row>
     <row r="7" spans="2:2">
@@ -14079,32 +14077,32 @@
     </row>
     <row r="10" spans="2:2">
       <c r="B10" s="131" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="11" spans="2:2">
       <c r="B11" s="55" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
     <row r="12" spans="2:2">
       <c r="B12" s="55" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
     </row>
     <row r="13" spans="2:2">
       <c r="B13" s="55" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="14" spans="2:2">
       <c r="B14" s="131" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="15" spans="2:2">
       <c r="B15" s="131" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
     </row>
     <row r="16" spans="2:2">
@@ -14634,33 +14632,33 @@
     <row r="15" spans="2:4" ht="47" customHeight="1">
       <c r="B15" s="38"/>
       <c r="C15" s="97" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D15" s="40"/>
     </row>
     <row r="16" spans="2:4" ht="47" customHeight="1">
       <c r="B16" s="38"/>
       <c r="C16" s="97" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="D16" s="40"/>
     </row>
     <row r="17" spans="2:4" ht="14" customHeight="1">
       <c r="B17" s="38"/>
       <c r="C17" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="D17" s="40" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="14" customHeight="1">
       <c r="B18" s="38"/>
       <c r="C18" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="D18" s="40" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="16" thickBot="1">
@@ -14957,7 +14955,7 @@
     </row>
     <row r="58" spans="2:4">
       <c r="B58" s="32" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="C58" s="142" t="s">
         <v>267</v>
@@ -15053,7 +15051,7 @@
     </row>
     <row r="74" spans="2:3">
       <c r="B74" s="37" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="C74" s="42" t="s">
         <v>269</v>
@@ -15428,7 +15426,7 @@
   </sheetPr>
   <dimension ref="B2:S67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -15456,7 +15454,7 @@
         <v>30</v>
       </c>
       <c r="K2" s="207" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="L2" s="13"/>
       <c r="M2" s="5"/>
@@ -15541,7 +15539,7 @@
       </c>
       <c r="F9" s="33"/>
       <c r="G9" s="33" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="H9" s="33"/>
       <c r="I9" s="33" t="s">
@@ -15558,10 +15556,10 @@
         <v>95</v>
       </c>
       <c r="O9" s="235" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="P9" s="236" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="10" spans="2:16">
@@ -15577,7 +15575,7 @@
       <c r="I10" s="15"/>
       <c r="J10" s="16"/>
       <c r="K10" s="372" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="L10" s="373" t="b">
         <f>IF(COUNTIF(P:P,0)+COUNTIF(P:P,FALSE)=0,TRUE,FALSE)</f>
@@ -15596,7 +15594,7 @@
       <c r="E11" s="311"/>
       <c r="F11" s="15"/>
       <c r="G11" s="230" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="H11" s="228"/>
       <c r="I11" s="15"/>
@@ -15610,7 +15608,7 @@
       </c>
       <c r="M11" s="65"/>
       <c r="O11" s="233" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="P11" s="234">
         <f>IF(L11=TRUE,1,0)</f>
@@ -15620,13 +15618,13 @@
     <row r="12" spans="2:16">
       <c r="B12" s="35"/>
       <c r="C12" s="60" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="D12" s="60"/>
       <c r="E12" s="311"/>
       <c r="F12" s="15"/>
       <c r="G12" s="230" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="H12" s="228"/>
       <c r="I12" s="15"/>
@@ -15635,7 +15633,7 @@
       <c r="L12" s="155"/>
       <c r="M12" s="65"/>
       <c r="O12" s="233" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="P12" s="234"/>
     </row>
@@ -15666,7 +15664,7 @@
       <c r="I14" s="15"/>
       <c r="J14" s="16"/>
       <c r="K14" s="64" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="L14" s="155"/>
       <c r="M14" s="65"/>
@@ -15684,7 +15682,7 @@
       <c r="I15" s="15"/>
       <c r="J15" s="16"/>
       <c r="K15" s="55" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="L15" s="380" t="e">
         <f>IF('Final demand per energy carrier'!E42&lt;0,FALSE,TRUE)</f>
@@ -15711,7 +15709,7 @@
       <c r="I16" s="15"/>
       <c r="J16" s="16"/>
       <c r="K16" s="55" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="L16" s="380" t="e">
         <f>IF('Final demand per energy carrier'!F42&lt;0,FALSE,TRUE)</f>
@@ -15738,7 +15736,7 @@
       <c r="I17" s="15"/>
       <c r="J17" s="16"/>
       <c r="K17" s="55" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="L17" s="380" t="e">
         <f>IF('Final demand per energy carrier'!G42&lt;0,FALSE,TRUE)</f>
@@ -15781,7 +15779,7 @@
       <c r="I19" s="317"/>
       <c r="J19" s="319"/>
       <c r="K19" s="320" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="L19" s="399" t="b">
         <f>IF('Fuel aggregation'!J11=0,TRUE,'Fuel aggregation'!J11)</f>
@@ -15815,10 +15813,10 @@
     <row r="21" spans="2:16">
       <c r="B21" s="37"/>
       <c r="C21" s="8" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="E21" s="213">
         <f>Final_demand_residences</f>
@@ -15828,7 +15826,7 @@
       <c r="G21" s="230"/>
       <c r="H21" s="230"/>
       <c r="I21" s="8" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="J21" s="8"/>
       <c r="K21" s="55"/>
@@ -15859,12 +15857,12 @@
         <v>103</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="E23" s="215"/>
       <c r="F23" s="230"/>
       <c r="G23" s="230" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="H23" s="230"/>
       <c r="I23" s="23"/>
@@ -15873,7 +15871,7 @@
       <c r="L23" s="375"/>
       <c r="M23" s="56"/>
       <c r="O23" s="233" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="P23" s="234"/>
     </row>
@@ -15883,12 +15881,12 @@
         <v>106</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="E24" s="216"/>
       <c r="F24" s="230"/>
       <c r="G24" s="230" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="H24" s="230"/>
       <c r="I24" s="23"/>
@@ -15897,7 +15895,7 @@
       <c r="L24" s="375"/>
       <c r="M24" s="56"/>
       <c r="O24" s="233" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="P24" s="234"/>
     </row>
@@ -15907,12 +15905,12 @@
         <v>104</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="E25" s="216"/>
       <c r="F25" s="230"/>
       <c r="G25" s="230" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="H25" s="230"/>
       <c r="I25" s="23"/>
@@ -15921,7 +15919,7 @@
       <c r="L25" s="375"/>
       <c r="M25" s="56"/>
       <c r="O25" s="233" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="P25" s="234"/>
     </row>
@@ -15947,7 +15945,7 @@
         <v>278</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="E27" s="376" t="e">
         <f>'Final demand per energy carrier'!J41</f>
@@ -15959,7 +15957,7 @@
       <c r="I27" s="8"/>
       <c r="J27" s="8"/>
       <c r="K27" s="64" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="L27" s="380" t="e">
         <f>IF(E27&gt;0,TRUE,E27)</f>
@@ -15978,10 +15976,10 @@
     <row r="28" spans="2:16">
       <c r="B28" s="37"/>
       <c r="C28" s="8" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="E28" s="377" t="e">
         <f>SUM('Final demand per energy carrier'!E42:G42)</f>
@@ -15993,7 +15991,7 @@
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
       <c r="K28" s="64" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="L28" s="380" t="e">
         <f>IF(E28&gt;0,TRUE,E28)</f>
@@ -16057,7 +16055,7 @@
     <row r="31" spans="2:16" ht="16" customHeight="1">
       <c r="B31" s="37"/>
       <c r="C31" s="8" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="D31" s="8"/>
       <c r="E31" s="376">
@@ -16094,7 +16092,7 @@
     <row r="33" spans="2:19">
       <c r="B33" s="37"/>
       <c r="C33" s="379" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="D33" s="8"/>
       <c r="E33" s="376">
@@ -16105,7 +16103,7 @@
       <c r="G33" s="224"/>
       <c r="H33" s="224"/>
       <c r="I33" s="8" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="J33" s="8"/>
       <c r="K33" s="55"/>
@@ -16117,7 +16115,7 @@
     <row r="34" spans="2:19">
       <c r="B34" s="37"/>
       <c r="C34" s="379" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="D34" s="8"/>
       <c r="E34" s="376">
@@ -16128,7 +16126,7 @@
       <c r="G34" s="224"/>
       <c r="H34" s="224"/>
       <c r="I34" s="8" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="J34" s="8"/>
       <c r="K34" s="55"/>
@@ -16140,7 +16138,7 @@
     <row r="35" spans="2:19">
       <c r="B35" s="37"/>
       <c r="C35" s="379" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="D35" s="8"/>
       <c r="E35" s="376">
@@ -16151,7 +16149,7 @@
       <c r="G35" s="224"/>
       <c r="H35" s="224"/>
       <c r="I35" s="8" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="J35" s="8"/>
       <c r="K35" s="55"/>
@@ -16179,7 +16177,7 @@
     <row r="37" spans="2:19" ht="30">
       <c r="B37" s="37"/>
       <c r="C37" s="378" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="D37" s="8"/>
       <c r="E37" s="376">
@@ -16216,7 +16214,7 @@
     <row r="39" spans="2:19" ht="16" thickBot="1">
       <c r="B39" s="37"/>
       <c r="C39" s="8" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="D39" s="8"/>
       <c r="E39" s="59"/>
@@ -16234,7 +16232,7 @@
     <row r="40" spans="2:19" ht="16" thickBot="1">
       <c r="B40" s="37"/>
       <c r="C40" s="379" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="D40" s="8"/>
       <c r="E40" s="171"/>
@@ -16247,14 +16245,14 @@
       <c r="L40" s="156"/>
       <c r="M40" s="314"/>
       <c r="O40" s="233" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="P40" s="234"/>
     </row>
     <row r="41" spans="2:19" ht="16" thickBot="1">
       <c r="B41" s="37"/>
       <c r="C41" s="379" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="D41" s="8"/>
       <c r="E41" s="171"/>
@@ -16267,7 +16265,7 @@
       <c r="L41" s="156"/>
       <c r="M41" s="314"/>
       <c r="O41" s="233" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="P41" s="234"/>
       <c r="S41" s="312"/>
@@ -16275,7 +16273,7 @@
     <row r="42" spans="2:19" ht="16" thickBot="1">
       <c r="B42" s="37"/>
       <c r="C42" s="379" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="D42" s="8"/>
       <c r="E42" s="171"/>
@@ -16288,14 +16286,14 @@
       <c r="L42" s="156"/>
       <c r="M42" s="314"/>
       <c r="O42" s="233" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="P42" s="234"/>
     </row>
     <row r="43" spans="2:19" ht="16" thickBot="1">
       <c r="B43" s="37"/>
       <c r="C43" s="379" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="D43" s="8"/>
       <c r="E43" s="171"/>
@@ -16308,14 +16306,14 @@
       <c r="L43" s="156"/>
       <c r="M43" s="56"/>
       <c r="O43" s="233" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="P43" s="234"/>
     </row>
     <row r="44" spans="2:19" ht="16" thickBot="1">
       <c r="B44" s="37"/>
       <c r="C44" s="379" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="D44" s="8"/>
       <c r="E44" s="171"/>
@@ -16328,14 +16326,14 @@
       <c r="L44" s="157"/>
       <c r="M44" s="56"/>
       <c r="O44" s="233" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="P44" s="234"/>
     </row>
     <row r="45" spans="2:19" ht="16" thickBot="1">
       <c r="B45" s="37"/>
       <c r="C45" s="379" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="D45" s="8"/>
       <c r="E45" s="171"/>
@@ -16348,7 +16346,7 @@
       <c r="L45" s="156"/>
       <c r="M45" s="56"/>
       <c r="O45" s="233" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="P45" s="234"/>
       <c r="R45" s="312"/>
@@ -16401,7 +16399,7 @@
     <row r="48" spans="2:19" ht="16" thickBot="1">
       <c r="B48" s="37"/>
       <c r="C48" s="60" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="D48" s="60"/>
       <c r="E48" s="63"/>
@@ -16419,7 +16417,7 @@
     <row r="49" spans="2:18" ht="16" thickBot="1">
       <c r="B49" s="37"/>
       <c r="C49" s="379" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="D49" s="8"/>
       <c r="E49" s="191"/>
@@ -16432,7 +16430,7 @@
       <c r="L49" s="156"/>
       <c r="M49" s="56"/>
       <c r="O49" s="233" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="P49" s="237"/>
       <c r="R49" s="312"/>
@@ -16440,7 +16438,7 @@
     <row r="50" spans="2:18" ht="16" thickBot="1">
       <c r="B50" s="37"/>
       <c r="C50" s="379" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="D50" s="8"/>
       <c r="E50" s="171"/>
@@ -16453,7 +16451,7 @@
       <c r="L50" s="156"/>
       <c r="M50" s="56"/>
       <c r="O50" s="233" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="P50" s="237"/>
     </row>
@@ -16473,7 +16471,7 @@
       <c r="L51" s="156"/>
       <c r="M51" s="56"/>
       <c r="O51" s="233" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="P51" s="237"/>
     </row>
@@ -16525,7 +16523,7 @@
     <row r="54" spans="2:18">
       <c r="B54" s="37"/>
       <c r="C54" s="8" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="D54" s="8"/>
       <c r="E54" s="59"/>
@@ -16558,7 +16556,7 @@
       <c r="L55" s="55"/>
       <c r="M55" s="56"/>
       <c r="O55" s="233" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="P55" s="237"/>
     </row>
@@ -16580,7 +16578,7 @@
       <c r="L56" s="55"/>
       <c r="M56" s="56"/>
       <c r="O56" s="233" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="P56" s="7"/>
     </row>
@@ -16600,7 +16598,7 @@
       <c r="L57" s="55"/>
       <c r="M57" s="56"/>
       <c r="O57" s="233" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="P57" s="7"/>
     </row>
@@ -16620,14 +16618,14 @@
       <c r="L58" s="55"/>
       <c r="M58" s="56"/>
       <c r="O58" s="233" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="P58" s="7"/>
     </row>
     <row r="59" spans="2:18" ht="16" thickBot="1">
       <c r="B59" s="37"/>
       <c r="C59" s="379" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="D59" s="8"/>
       <c r="E59" s="171"/>
@@ -16640,7 +16638,7 @@
       <c r="L59" s="55"/>
       <c r="M59" s="56"/>
       <c r="O59" s="233" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="P59" s="7"/>
     </row>
@@ -16662,7 +16660,7 @@
     </row>
     <row r="61" spans="2:18">
       <c r="B61" s="302" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="C61" s="53"/>
       <c r="D61" s="53"/>
@@ -16681,7 +16679,7 @@
     <row r="62" spans="2:18">
       <c r="B62" s="30"/>
       <c r="C62" s="8" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="D62" s="8"/>
       <c r="E62" s="172">
@@ -16695,14 +16693,14 @@
       <c r="L62" s="8"/>
       <c r="M62" s="31"/>
       <c r="O62" s="233" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="P62" s="7"/>
     </row>
     <row r="63" spans="2:18">
       <c r="B63" s="30"/>
       <c r="C63" s="8" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="D63" s="8"/>
       <c r="E63" s="172">
@@ -16716,7 +16714,7 @@
       <c r="L63" s="8"/>
       <c r="M63" s="31"/>
       <c r="O63" s="233" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="P63" s="7"/>
     </row>
@@ -16738,7 +16736,7 @@
     <row r="65" spans="2:16">
       <c r="B65" s="30"/>
       <c r="C65" s="8" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="D65" s="8"/>
       <c r="E65" s="172">
@@ -16752,14 +16750,14 @@
       <c r="L65" s="8"/>
       <c r="M65" s="31"/>
       <c r="O65" s="233" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="P65" s="7"/>
     </row>
     <row r="66" spans="2:16">
       <c r="B66" s="30"/>
       <c r="C66" s="8" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="D66" s="8"/>
       <c r="E66" s="172">
@@ -16773,7 +16771,7 @@
       <c r="L66" s="8"/>
       <c r="M66" s="31"/>
       <c r="O66" s="233" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="P66" s="7"/>
     </row>
@@ -16954,7 +16952,7 @@
   <sheetData>
     <row r="2" spans="2:67" ht="20">
       <c r="B2" s="2" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
     </row>
     <row r="3" spans="2:67" ht="15" customHeight="1">
@@ -23828,7 +23826,7 @@
     </row>
     <row r="5" spans="2:13">
       <c r="B5" s="403" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="C5" s="404"/>
       <c r="D5" s="404"/>
@@ -23853,15 +23851,15 @@
     </row>
     <row r="7" spans="2:13">
       <c r="B7" s="324" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="C7" s="325"/>
       <c r="D7" s="325"/>
       <c r="E7" s="326" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="F7" s="322" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="G7" s="321"/>
       <c r="H7" s="322"/>
@@ -23870,7 +23868,7 @@
       <c r="K7" s="329"/>
       <c r="L7" s="333"/>
       <c r="M7" s="258" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="8" spans="2:13" ht="30">
@@ -23882,19 +23880,19 @@
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="347" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="I8" s="331" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="J8" s="334" t="s">
         <v>232</v>
@@ -23912,16 +23910,16 @@
       <c r="D9" s="74"/>
       <c r="E9" s="332"/>
       <c r="F9" s="323" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="G9" s="323" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="H9" s="323" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="10"/>
@@ -23949,17 +23947,17 @@
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="345" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="F11" s="355"/>
       <c r="G11" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="H11" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="I11" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="J11" s="366">
         <f>F11</f>
@@ -23971,7 +23969,7 @@
         <v>0</v>
       </c>
       <c r="M11" s="258" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="12" spans="2:13">
@@ -23981,15 +23979,15 @@
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="345" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="F12" s="355"/>
       <c r="G12" s="355"/>
       <c r="H12" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="I12" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="J12" s="366"/>
       <c r="K12" s="360" t="e">
@@ -24001,7 +23999,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M12" s="258" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
     </row>
     <row r="13" spans="2:13">
@@ -24011,15 +24009,15 @@
       </c>
       <c r="D13" s="17"/>
       <c r="E13" s="345" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="F13" s="355"/>
       <c r="G13" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="H13" s="355"/>
       <c r="I13" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="J13" s="366"/>
       <c r="K13" s="360" t="e">
@@ -24031,7 +24029,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M13" s="258" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="14" spans="2:13">
@@ -24041,17 +24039,17 @@
       </c>
       <c r="D14" s="17"/>
       <c r="E14" s="345" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="F14" s="355"/>
       <c r="G14" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="H14" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="I14" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="J14" s="366">
         <f>F14</f>
@@ -24063,7 +24061,7 @@
         <v>0</v>
       </c>
       <c r="M14" s="258" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
     </row>
     <row r="15" spans="2:13">
@@ -24073,17 +24071,17 @@
       </c>
       <c r="D15" s="17"/>
       <c r="E15" s="345" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="F15" s="355"/>
       <c r="G15" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="H15" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="I15" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="J15" s="366">
         <f>F15</f>
@@ -24095,7 +24093,7 @@
         <v>0</v>
       </c>
       <c r="M15" s="258" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
     </row>
     <row r="16" spans="2:13">
@@ -24105,17 +24103,17 @@
       </c>
       <c r="D16" s="17"/>
       <c r="E16" s="345" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="F16" s="355"/>
       <c r="G16" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="H16" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="I16" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="J16" s="366">
         <f>F16</f>
@@ -24127,7 +24125,7 @@
         <v>0</v>
       </c>
       <c r="M16" s="258" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
     </row>
     <row r="17" spans="2:13">
@@ -24149,17 +24147,17 @@
       </c>
       <c r="D18" s="17"/>
       <c r="E18" s="345" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="F18" s="355"/>
       <c r="G18" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="H18" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="I18" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="J18" s="366">
         <f>F18</f>
@@ -24171,7 +24169,7 @@
         <v>0</v>
       </c>
       <c r="M18" s="258" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
     </row>
     <row r="19" spans="2:13">
@@ -24181,17 +24179,17 @@
       </c>
       <c r="D19" s="17"/>
       <c r="E19" s="345" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="F19" s="355"/>
       <c r="G19" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="H19" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="I19" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="J19" s="366">
         <f>F19</f>
@@ -24203,7 +24201,7 @@
         <v>0</v>
       </c>
       <c r="M19" s="258" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
     </row>
     <row r="20" spans="2:13">
@@ -24213,17 +24211,17 @@
       </c>
       <c r="D20" s="17"/>
       <c r="E20" s="345" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="F20" s="355"/>
       <c r="G20" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="H20" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="I20" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="J20" s="366">
         <f>F20</f>
@@ -24235,7 +24233,7 @@
         <v>0</v>
       </c>
       <c r="M20" s="258" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
     </row>
     <row r="21" spans="2:13">
@@ -24274,17 +24272,17 @@
       </c>
       <c r="D23" s="17"/>
       <c r="E23" s="345" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="F23" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="G23" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="H23" s="355"/>
       <c r="I23" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="J23" s="366"/>
       <c r="K23" s="360" t="e">
@@ -24296,7 +24294,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M23" s="258" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
     </row>
     <row r="24" spans="2:13">
@@ -24306,17 +24304,17 @@
       </c>
       <c r="D24" s="17"/>
       <c r="E24" s="345" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="F24" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="G24" s="355"/>
       <c r="H24" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="I24" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="J24" s="366"/>
       <c r="K24" s="360" t="e">
@@ -24328,7 +24326,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M24" s="258" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
     </row>
     <row r="25" spans="2:13">
@@ -24338,17 +24336,17 @@
       </c>
       <c r="D25" s="17"/>
       <c r="E25" s="345" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="F25" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="G25" s="355"/>
       <c r="H25" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="I25" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="J25" s="366"/>
       <c r="K25" s="360" t="e">
@@ -24360,7 +24358,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M25" s="258" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
     </row>
     <row r="26" spans="2:13">
@@ -24411,7 +24409,7 @@
         <v>0.05</v>
       </c>
       <c r="M28" s="258" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
     <row r="29" spans="2:13">
@@ -24434,7 +24432,7 @@
         <v>0.12</v>
       </c>
       <c r="M29" s="258" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
     </row>
     <row r="30" spans="2:13">
@@ -24444,16 +24442,16 @@
       </c>
       <c r="D30" s="17"/>
       <c r="E30" s="345" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="F30" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="G30" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="H30" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="I30" s="355"/>
       <c r="J30" s="366">
@@ -24466,7 +24464,7 @@
         <v>0</v>
       </c>
       <c r="M30" s="258" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
     </row>
     <row r="31" spans="2:13">
@@ -24476,16 +24474,16 @@
       </c>
       <c r="D31" s="17"/>
       <c r="E31" s="345" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="F31" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="G31" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="H31" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="I31" s="355"/>
       <c r="J31" s="366">
@@ -24498,7 +24496,7 @@
         <v>0</v>
       </c>
       <c r="M31" s="258" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="32" spans="2:13">
@@ -24508,16 +24506,16 @@
       </c>
       <c r="D32" s="17"/>
       <c r="E32" s="345" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="F32" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="G32" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="H32" s="355" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="I32" s="355"/>
       <c r="J32" s="366">
@@ -24530,7 +24528,7 @@
         <v>0</v>
       </c>
       <c r="M32" s="258" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
     </row>
     <row r="33" spans="2:12" ht="16" thickBot="1">

</xml_diff>

<commit_message>
Published state of ETDataset on 4 December 2015
</commit_message>
<xml_diff>
--- a/analyses/7_services_analysis.xlsx
+++ b/analyses/7_services_analysis.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15960" tabRatio="929" firstSheet="15" activeTab="19"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="38400" windowHeight="23460" tabRatio="929" firstSheet="10" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="34" r:id="rId1"/>
@@ -62,7 +62,7 @@
     <definedName name="Final_demand_space_cooling">Dashboard!$E$24</definedName>
     <definedName name="Final_demand_space_heating">Dashboard!$E$23</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000" iterate="1" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -180,7 +180,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="610">
   <si>
     <t>Changelog</t>
   </si>
@@ -1467,9 +1467,6 @@
   </si>
   <si>
     <t>buildings_cooling_collective_heatpump_water_water_ts_electricity</t>
-  </si>
-  <si>
-    <t>buildings_cooling_collective_cooling_network_electricity</t>
   </si>
   <si>
     <t>buildings_final_demand_for_cooling_electricity</t>
@@ -9603,13 +9600,13 @@
     <row r="6" spans="2:5" ht="16" thickBot="1"/>
     <row r="7" spans="2:5" ht="30">
       <c r="B7" s="201" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C7" s="283" t="s">
         <v>341</v>
       </c>
       <c r="D7" s="167" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E7" s="168" t="s">
         <v>346</v>
@@ -9659,7 +9656,7 @@
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="279" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C12" s="169"/>
       <c r="D12" s="223"/>
@@ -9888,10 +9885,10 @@
     <row r="6" spans="2:6" ht="16" thickBot="1"/>
     <row r="7" spans="2:6" ht="30">
       <c r="B7" s="201" t="s">
+        <v>490</v>
+      </c>
+      <c r="C7" s="274" t="s">
         <v>491</v>
-      </c>
-      <c r="C7" s="274" t="s">
-        <v>492</v>
       </c>
       <c r="D7" s="283" t="s">
         <v>229</v>
@@ -9900,7 +9897,7 @@
         <v>351</v>
       </c>
       <c r="F7" s="168" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="8" spans="2:6">
@@ -9915,7 +9912,7 @@
     <row r="9" spans="2:6">
       <c r="B9" s="280"/>
       <c r="C9" s="60" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>123</v>
@@ -9954,7 +9951,7 @@
     <row r="12" spans="2:6">
       <c r="B12" s="280"/>
       <c r="C12" s="60" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>125</v>
@@ -10002,7 +9999,7 @@
     <row r="16" spans="2:6">
       <c r="B16" s="280"/>
       <c r="C16" s="60" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>125</v>
@@ -10050,7 +10047,7 @@
     <row r="20" spans="2:6">
       <c r="B20" s="280"/>
       <c r="C20" s="60" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>134</v>
@@ -10205,7 +10202,7 @@
     </row>
     <row r="5" spans="1:11" ht="30" customHeight="1">
       <c r="B5" s="400" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C5" s="402"/>
       <c r="D5" s="402"/>
@@ -10263,28 +10260,28 @@
         <v>132</v>
       </c>
       <c r="D9" s="108" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E9" s="69" t="s">
+        <v>483</v>
+      </c>
+      <c r="F9" s="69" t="s">
+        <v>601</v>
+      </c>
+      <c r="G9" s="69" t="s">
         <v>484</v>
       </c>
-      <c r="F9" s="69" t="s">
-        <v>602</v>
-      </c>
-      <c r="G9" s="69" t="s">
+      <c r="H9" s="69" t="s">
         <v>485</v>
       </c>
-      <c r="H9" s="69" t="s">
+      <c r="I9" s="69" t="s">
         <v>486</v>
       </c>
-      <c r="I9" s="69" t="s">
+      <c r="J9" s="69" t="s">
         <v>487</v>
       </c>
-      <c r="J9" s="69" t="s">
+      <c r="K9" s="146" t="s">
         <v>488</v>
-      </c>
-      <c r="K9" s="146" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -10804,7 +10801,7 @@
     <row r="38" spans="2:12">
       <c r="B38" s="30"/>
       <c r="C38" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D38" s="75"/>
       <c r="E38" s="257" t="e">
@@ -10851,7 +10848,7 @@
     </row>
     <row r="40" spans="2:12">
       <c r="B40" s="396" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="5"/>
@@ -10883,7 +10880,7 @@
     <row r="42" spans="2:12">
       <c r="B42" s="30"/>
       <c r="C42" s="17" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D42" s="75"/>
       <c r="E42" s="257" t="e">
@@ -10899,16 +10896,16 @@
         <v>#DIV/0!</v>
       </c>
       <c r="H42" s="383" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="I42" s="383" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="J42" s="383" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="K42" s="391" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="43" spans="2:12" ht="16" thickBot="1">
@@ -10995,7 +10992,7 @@
     <row r="6" spans="2:10" ht="16" thickBot="1"/>
     <row r="7" spans="2:10">
       <c r="B7" s="27" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C7" s="53"/>
       <c r="D7" s="28"/>
@@ -11757,7 +11754,7 @@
         <v>274</v>
       </c>
       <c r="D9" s="69" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E9" s="69" t="s">
         <v>275</v>
@@ -11778,10 +11775,10 @@
         <v>290</v>
       </c>
       <c r="K9" s="265" t="s">
+        <v>474</v>
+      </c>
+      <c r="L9" s="146" t="s">
         <v>475</v>
-      </c>
-      <c r="L9" s="146" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="10" spans="2:13">
@@ -11869,13 +11866,13 @@
     </row>
     <row r="17" spans="10:11">
       <c r="J17" s="259" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K17" s="203"/>
     </row>
     <row r="18" spans="10:11">
       <c r="J18" s="260" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="K18" s="261"/>
     </row>
@@ -11895,13 +11892,13 @@
     </row>
     <row r="21" spans="10:11">
       <c r="J21" s="260" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="K21" s="261"/>
     </row>
     <row r="22" spans="10:11">
       <c r="J22" s="260" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="K22" s="261"/>
     </row>
@@ -11911,7 +11908,7 @@
     </row>
     <row r="24" spans="10:11">
       <c r="J24" s="262" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K24" s="263">
         <f>K11-Final_demand_residences</f>
@@ -12021,10 +12018,10 @@
         <v>301</v>
       </c>
       <c r="E8" s="108" t="s">
+        <v>425</v>
+      </c>
+      <c r="F8" s="108" t="s">
         <v>426</v>
-      </c>
-      <c r="F8" s="108" t="s">
-        <v>427</v>
       </c>
       <c r="G8" s="190" t="s">
         <v>302</v>
@@ -12455,8 +12452,8 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -12467,7 +12464,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="205" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -12497,12 +12494,8 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="241" t="s">
-        <v>386</v>
-      </c>
-      <c r="B5" s="284">
-        <v>0</v>
-      </c>
+      <c r="A5" s="241"/>
+      <c r="B5" s="284"/>
     </row>
     <row r="6" spans="1:2">
       <c r="B6" s="284"/>
@@ -12771,7 +12764,7 @@
         <v>41485</v>
       </c>
       <c r="C23" s="39" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D23" s="309">
         <v>1.18</v>
@@ -12783,7 +12776,7 @@
         <v>41485</v>
       </c>
       <c r="C24" s="39" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D24" s="309">
         <v>1.18</v>
@@ -12795,7 +12788,7 @@
         <v>41486</v>
       </c>
       <c r="C25" s="39" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D25" s="309">
         <v>1.19</v>
@@ -12807,7 +12800,7 @@
         <v>41487</v>
       </c>
       <c r="C26" s="39" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D26" s="309">
         <v>1.19</v>
@@ -12819,7 +12812,7 @@
         <v>41499</v>
       </c>
       <c r="C27" s="39" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D27" s="308">
         <v>1.2</v>
@@ -12831,7 +12824,7 @@
         <v>41500</v>
       </c>
       <c r="C28" s="39" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D28" s="309">
         <v>1.21</v>
@@ -12843,7 +12836,7 @@
         <v>41500</v>
       </c>
       <c r="C29" s="39" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D29" s="308">
         <v>1.22</v>
@@ -12855,7 +12848,7 @@
         <v>41502</v>
       </c>
       <c r="C30" s="39" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D30" s="308">
         <v>1.23</v>
@@ -12867,7 +12860,7 @@
         <v>41505</v>
       </c>
       <c r="C31" s="39" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D31" s="308">
         <v>1.24</v>
@@ -12879,7 +12872,7 @@
         <v>41506</v>
       </c>
       <c r="C32" s="39" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D32" s="308">
         <v>1.25</v>
@@ -12891,7 +12884,7 @@
         <v>41507</v>
       </c>
       <c r="C33" s="39" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D33" s="308">
         <v>1.26</v>
@@ -12903,7 +12896,7 @@
         <v>41509</v>
       </c>
       <c r="C34" s="39" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D34" s="308">
         <v>1.27</v>
@@ -12915,7 +12908,7 @@
         <v>41509</v>
       </c>
       <c r="C35" s="39" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D35" s="308">
         <v>1.28</v>
@@ -12924,10 +12917,10 @@
     </row>
     <row r="36" spans="2:5">
       <c r="B36" s="305" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C36" s="39" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D36" s="308">
         <v>1.29</v>
@@ -12939,7 +12932,7 @@
         <v>41534</v>
       </c>
       <c r="C37" s="39" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D37" s="308">
         <v>1.3</v>
@@ -12951,7 +12944,7 @@
         <v>41542</v>
       </c>
       <c r="C38" s="39" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D38" s="308">
         <v>1.31</v>
@@ -12963,7 +12956,7 @@
         <v>41562</v>
       </c>
       <c r="C39" s="371" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D39" s="308">
         <v>1.32</v>
@@ -12975,7 +12968,7 @@
         <v>41578</v>
       </c>
       <c r="C40" s="39" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D40" s="308">
         <v>1.33</v>
@@ -12987,7 +12980,7 @@
         <v>41578</v>
       </c>
       <c r="C41" s="39" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D41" s="308">
         <v>1.34</v>
@@ -12999,7 +12992,7 @@
         <v>41782</v>
       </c>
       <c r="C42" s="39" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="D42" s="308">
         <v>1.35</v>
@@ -13011,7 +13004,7 @@
         <v>41782</v>
       </c>
       <c r="C43" s="39" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D43" s="308">
         <v>1.36</v>
@@ -13070,7 +13063,7 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A3" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -13079,7 +13072,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="205" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -13092,7 +13085,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="205" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B3" s="284" t="e">
         <f>'Technology shares'!F9</f>
@@ -13101,7 +13094,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="205" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B4" s="284" t="e">
         <f>'Technology shares'!F10</f>
@@ -13146,7 +13139,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="205" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -13159,7 +13152,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="205" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B3" s="284" t="e">
         <f>'Application shares'!E9</f>
@@ -13168,7 +13161,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="205" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B4" s="284" t="e">
         <f>'Application shares'!E10</f>
@@ -13213,7 +13206,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="205" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -13226,7 +13219,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="205" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B3" s="284" t="e">
         <f>'Application shares'!E13</f>
@@ -13235,7 +13228,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="205" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B4" s="284" t="e">
         <f>'Application shares'!E14</f>
@@ -13244,7 +13237,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="205" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B5" s="284" t="e">
         <f>'Application shares'!E15</f>
@@ -13286,7 +13279,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="205" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -13299,7 +13292,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="205" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B3" s="284" t="e">
         <f>'Application shares'!E18</f>
@@ -13308,7 +13301,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="205" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B4" s="284" t="e">
         <f>'Application shares'!E19</f>
@@ -13353,7 +13346,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="205" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -13375,7 +13368,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="205" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B4" s="284" t="e">
         <f>'Application shares'!E23</f>
@@ -13393,7 +13386,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="205" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B6" s="284" t="e">
         <f>'Application shares'!E25</f>
@@ -13432,7 +13425,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="205" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -13445,7 +13438,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="205" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B3" s="284">
         <f>Dashboard!E62</f>
@@ -13454,7 +13447,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="205" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B4" s="284">
         <f>Dashboard!E63</f>
@@ -13500,7 +13493,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -13513,7 +13506,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B3" s="284">
         <v>0</v>
@@ -13521,7 +13514,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B4" s="284">
         <v>1</v>
@@ -13566,7 +13559,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -13579,7 +13572,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B3" s="284">
         <v>0</v>
@@ -13587,7 +13580,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B4" s="284">
         <v>1</v>
@@ -13632,7 +13625,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -13645,7 +13638,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B3" s="284">
         <f>1-B4</f>
@@ -13654,7 +13647,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B4" s="284">
         <f>Dashboard!E65</f>
@@ -13700,7 +13693,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -13713,7 +13706,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B3" s="284">
         <f>1-B4</f>
@@ -13722,7 +13715,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B4" s="284">
         <f>Dashboard!E66</f>
@@ -13843,7 +13836,7 @@
     </row>
     <row r="13" spans="2:3" ht="28" customHeight="1">
       <c r="B13" s="177" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C13" s="61" t="s">
         <v>321</v>
@@ -13859,7 +13852,7 @@
     </row>
     <row r="15" spans="2:3" ht="28" customHeight="1">
       <c r="B15" s="300" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C15" s="61" t="s">
         <v>347</v>
@@ -13867,7 +13860,7 @@
     </row>
     <row r="16" spans="2:3" ht="28" customHeight="1">
       <c r="B16" s="300" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C16" s="61" t="s">
         <v>345</v>
@@ -13883,7 +13876,7 @@
     </row>
     <row r="18" spans="2:3" ht="28" customHeight="1">
       <c r="B18" s="126" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C18" s="61" t="s">
         <v>319</v>
@@ -13894,7 +13887,7 @@
         <v>317</v>
       </c>
       <c r="C19" s="61" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="28" customHeight="1">
@@ -13915,106 +13908,106 @@
     </row>
     <row r="22" spans="2:3" ht="28" customHeight="1">
       <c r="B22" s="178" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C22" s="256" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="28" customHeight="1">
       <c r="B23" s="178" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C23" s="256" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="24" spans="2:3" ht="28" customHeight="1">
       <c r="B24" s="178" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C24" s="256" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="28" customHeight="1">
       <c r="B25" s="178" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C25" s="256" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="26" spans="2:3" ht="28" customHeight="1">
       <c r="B26" s="178" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C26" s="256" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="27" spans="2:3" ht="28" customHeight="1">
       <c r="B27" s="178" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C27" s="256" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="28" spans="2:3" ht="28" customHeight="1">
       <c r="B28" s="178" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C28" s="256" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="29" spans="2:3" ht="28" customHeight="1">
       <c r="B29" s="178" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C29" s="256" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="30" spans="2:3" ht="28" customHeight="1">
       <c r="B30" s="178" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C30" s="256" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="31" spans="2:3" ht="28" customHeight="1">
       <c r="B31" s="178" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C31" s="256" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="32" spans="2:3" ht="28" customHeight="1">
       <c r="B32" s="178" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C32" s="256" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="33" spans="2:3" ht="28" customHeight="1">
       <c r="B33" s="178" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C33" s="256" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="28" customHeight="1">
       <c r="B34" s="178" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C34" s="256" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="35" spans="2:3" ht="28" customHeight="1"/>
@@ -14061,7 +14054,7 @@
     </row>
     <row r="6" spans="2:2" ht="75">
       <c r="B6" s="113" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="7" spans="2:2">
@@ -14077,32 +14070,32 @@
     </row>
     <row r="10" spans="2:2">
       <c r="B10" s="131" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="11" spans="2:2">
       <c r="B11" s="55" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="12" spans="2:2">
       <c r="B12" s="55" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="13" spans="2:2">
       <c r="B13" s="55" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="14" spans="2:2">
       <c r="B14" s="131" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="15" spans="2:2">
       <c r="B15" s="131" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="16" spans="2:2">
@@ -14632,33 +14625,33 @@
     <row r="15" spans="2:4" ht="47" customHeight="1">
       <c r="B15" s="38"/>
       <c r="C15" s="97" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D15" s="40"/>
     </row>
     <row r="16" spans="2:4" ht="47" customHeight="1">
       <c r="B16" s="38"/>
       <c r="C16" s="97" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D16" s="40"/>
     </row>
     <row r="17" spans="2:4" ht="14" customHeight="1">
       <c r="B17" s="38"/>
       <c r="C17" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D17" s="40" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="14" customHeight="1">
       <c r="B18" s="38"/>
       <c r="C18" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D18" s="40" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="16" thickBot="1">
@@ -14955,7 +14948,7 @@
     </row>
     <row r="58" spans="2:4">
       <c r="B58" s="32" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C58" s="142" t="s">
         <v>267</v>
@@ -15051,7 +15044,7 @@
     </row>
     <row r="74" spans="2:3">
       <c r="B74" s="37" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C74" s="42" t="s">
         <v>269</v>
@@ -15454,7 +15447,7 @@
         <v>30</v>
       </c>
       <c r="K2" s="207" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="L2" s="13"/>
       <c r="M2" s="5"/>
@@ -15539,7 +15532,7 @@
       </c>
       <c r="F9" s="33"/>
       <c r="G9" s="33" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H9" s="33"/>
       <c r="I9" s="33" t="s">
@@ -15556,10 +15549,10 @@
         <v>95</v>
       </c>
       <c r="O9" s="235" t="s">
+        <v>431</v>
+      </c>
+      <c r="P9" s="236" t="s">
         <v>432</v>
-      </c>
-      <c r="P9" s="236" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="10" spans="2:16">
@@ -15575,7 +15568,7 @@
       <c r="I10" s="15"/>
       <c r="J10" s="16"/>
       <c r="K10" s="372" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="L10" s="373" t="b">
         <f>IF(COUNTIF(P:P,0)+COUNTIF(P:P,FALSE)=0,TRUE,FALSE)</f>
@@ -15594,7 +15587,7 @@
       <c r="E11" s="311"/>
       <c r="F11" s="15"/>
       <c r="G11" s="230" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H11" s="228"/>
       <c r="I11" s="15"/>
@@ -15608,7 +15601,7 @@
       </c>
       <c r="M11" s="65"/>
       <c r="O11" s="233" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="P11" s="234">
         <f>IF(L11=TRUE,1,0)</f>
@@ -15618,13 +15611,13 @@
     <row r="12" spans="2:16">
       <c r="B12" s="35"/>
       <c r="C12" s="60" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D12" s="60"/>
       <c r="E12" s="311"/>
       <c r="F12" s="15"/>
       <c r="G12" s="230" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H12" s="228"/>
       <c r="I12" s="15"/>
@@ -15633,7 +15626,7 @@
       <c r="L12" s="155"/>
       <c r="M12" s="65"/>
       <c r="O12" s="233" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="P12" s="234"/>
     </row>
@@ -15664,7 +15657,7 @@
       <c r="I14" s="15"/>
       <c r="J14" s="16"/>
       <c r="K14" s="64" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="L14" s="155"/>
       <c r="M14" s="65"/>
@@ -15682,7 +15675,7 @@
       <c r="I15" s="15"/>
       <c r="J15" s="16"/>
       <c r="K15" s="55" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L15" s="380" t="e">
         <f>IF('Final demand per energy carrier'!E42&lt;0,FALSE,TRUE)</f>
@@ -15709,7 +15702,7 @@
       <c r="I16" s="15"/>
       <c r="J16" s="16"/>
       <c r="K16" s="55" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="L16" s="380" t="e">
         <f>IF('Final demand per energy carrier'!F42&lt;0,FALSE,TRUE)</f>
@@ -15736,7 +15729,7 @@
       <c r="I17" s="15"/>
       <c r="J17" s="16"/>
       <c r="K17" s="55" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="L17" s="380" t="e">
         <f>IF('Final demand per energy carrier'!G42&lt;0,FALSE,TRUE)</f>
@@ -15779,7 +15772,7 @@
       <c r="I19" s="317"/>
       <c r="J19" s="319"/>
       <c r="K19" s="320" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="L19" s="399" t="b">
         <f>IF('Fuel aggregation'!J11=0,TRUE,'Fuel aggregation'!J11)</f>
@@ -15813,10 +15806,10 @@
     <row r="21" spans="2:16">
       <c r="B21" s="37"/>
       <c r="C21" s="8" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E21" s="213">
         <f>Final_demand_residences</f>
@@ -15826,7 +15819,7 @@
       <c r="G21" s="230"/>
       <c r="H21" s="230"/>
       <c r="I21" s="8" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="J21" s="8"/>
       <c r="K21" s="55"/>
@@ -15857,12 +15850,12 @@
         <v>103</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E23" s="215"/>
       <c r="F23" s="230"/>
       <c r="G23" s="230" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H23" s="230"/>
       <c r="I23" s="23"/>
@@ -15871,7 +15864,7 @@
       <c r="L23" s="375"/>
       <c r="M23" s="56"/>
       <c r="O23" s="233" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="P23" s="234"/>
     </row>
@@ -15881,12 +15874,12 @@
         <v>106</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E24" s="216"/>
       <c r="F24" s="230"/>
       <c r="G24" s="230" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H24" s="230"/>
       <c r="I24" s="23"/>
@@ -15895,7 +15888,7 @@
       <c r="L24" s="375"/>
       <c r="M24" s="56"/>
       <c r="O24" s="233" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="P24" s="234"/>
     </row>
@@ -15905,12 +15898,12 @@
         <v>104</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E25" s="216"/>
       <c r="F25" s="230"/>
       <c r="G25" s="230" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H25" s="230"/>
       <c r="I25" s="23"/>
@@ -15919,7 +15912,7 @@
       <c r="L25" s="375"/>
       <c r="M25" s="56"/>
       <c r="O25" s="233" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="P25" s="234"/>
     </row>
@@ -15945,7 +15938,7 @@
         <v>278</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E27" s="376" t="e">
         <f>'Final demand per energy carrier'!J41</f>
@@ -15957,7 +15950,7 @@
       <c r="I27" s="8"/>
       <c r="J27" s="8"/>
       <c r="K27" s="64" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="L27" s="380" t="e">
         <f>IF(E27&gt;0,TRUE,E27)</f>
@@ -15976,10 +15969,10 @@
     <row r="28" spans="2:16">
       <c r="B28" s="37"/>
       <c r="C28" s="8" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E28" s="377" t="e">
         <f>SUM('Final demand per energy carrier'!E42:G42)</f>
@@ -15991,7 +15984,7 @@
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
       <c r="K28" s="64" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="L28" s="380" t="e">
         <f>IF(E28&gt;0,TRUE,E28)</f>
@@ -16055,7 +16048,7 @@
     <row r="31" spans="2:16" ht="16" customHeight="1">
       <c r="B31" s="37"/>
       <c r="C31" s="8" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D31" s="8"/>
       <c r="E31" s="376">
@@ -16092,7 +16085,7 @@
     <row r="33" spans="2:19">
       <c r="B33" s="37"/>
       <c r="C33" s="379" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D33" s="8"/>
       <c r="E33" s="376">
@@ -16103,7 +16096,7 @@
       <c r="G33" s="224"/>
       <c r="H33" s="224"/>
       <c r="I33" s="8" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="J33" s="8"/>
       <c r="K33" s="55"/>
@@ -16115,7 +16108,7 @@
     <row r="34" spans="2:19">
       <c r="B34" s="37"/>
       <c r="C34" s="379" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D34" s="8"/>
       <c r="E34" s="376">
@@ -16126,7 +16119,7 @@
       <c r="G34" s="224"/>
       <c r="H34" s="224"/>
       <c r="I34" s="8" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="J34" s="8"/>
       <c r="K34" s="55"/>
@@ -16138,7 +16131,7 @@
     <row r="35" spans="2:19">
       <c r="B35" s="37"/>
       <c r="C35" s="379" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D35" s="8"/>
       <c r="E35" s="376">
@@ -16149,7 +16142,7 @@
       <c r="G35" s="224"/>
       <c r="H35" s="224"/>
       <c r="I35" s="8" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="J35" s="8"/>
       <c r="K35" s="55"/>
@@ -16177,7 +16170,7 @@
     <row r="37" spans="2:19" ht="30">
       <c r="B37" s="37"/>
       <c r="C37" s="378" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D37" s="8"/>
       <c r="E37" s="376">
@@ -16214,7 +16207,7 @@
     <row r="39" spans="2:19" ht="16" thickBot="1">
       <c r="B39" s="37"/>
       <c r="C39" s="8" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D39" s="8"/>
       <c r="E39" s="59"/>
@@ -16232,7 +16225,7 @@
     <row r="40" spans="2:19" ht="16" thickBot="1">
       <c r="B40" s="37"/>
       <c r="C40" s="379" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D40" s="8"/>
       <c r="E40" s="171"/>
@@ -16245,14 +16238,14 @@
       <c r="L40" s="156"/>
       <c r="M40" s="314"/>
       <c r="O40" s="233" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="P40" s="234"/>
     </row>
     <row r="41" spans="2:19" ht="16" thickBot="1">
       <c r="B41" s="37"/>
       <c r="C41" s="379" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D41" s="8"/>
       <c r="E41" s="171"/>
@@ -16265,7 +16258,7 @@
       <c r="L41" s="156"/>
       <c r="M41" s="314"/>
       <c r="O41" s="233" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="P41" s="234"/>
       <c r="S41" s="312"/>
@@ -16273,7 +16266,7 @@
     <row r="42" spans="2:19" ht="16" thickBot="1">
       <c r="B42" s="37"/>
       <c r="C42" s="379" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D42" s="8"/>
       <c r="E42" s="171"/>
@@ -16286,14 +16279,14 @@
       <c r="L42" s="156"/>
       <c r="M42" s="314"/>
       <c r="O42" s="233" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="P42" s="234"/>
     </row>
     <row r="43" spans="2:19" ht="16" thickBot="1">
       <c r="B43" s="37"/>
       <c r="C43" s="379" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D43" s="8"/>
       <c r="E43" s="171"/>
@@ -16306,14 +16299,14 @@
       <c r="L43" s="156"/>
       <c r="M43" s="56"/>
       <c r="O43" s="233" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="P43" s="234"/>
     </row>
     <row r="44" spans="2:19" ht="16" thickBot="1">
       <c r="B44" s="37"/>
       <c r="C44" s="379" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D44" s="8"/>
       <c r="E44" s="171"/>
@@ -16326,14 +16319,14 @@
       <c r="L44" s="157"/>
       <c r="M44" s="56"/>
       <c r="O44" s="233" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="P44" s="234"/>
     </row>
     <row r="45" spans="2:19" ht="16" thickBot="1">
       <c r="B45" s="37"/>
       <c r="C45" s="379" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D45" s="8"/>
       <c r="E45" s="171"/>
@@ -16346,7 +16339,7 @@
       <c r="L45" s="156"/>
       <c r="M45" s="56"/>
       <c r="O45" s="233" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="P45" s="234"/>
       <c r="R45" s="312"/>
@@ -16399,7 +16392,7 @@
     <row r="48" spans="2:19" ht="16" thickBot="1">
       <c r="B48" s="37"/>
       <c r="C48" s="60" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D48" s="60"/>
       <c r="E48" s="63"/>
@@ -16417,7 +16410,7 @@
     <row r="49" spans="2:18" ht="16" thickBot="1">
       <c r="B49" s="37"/>
       <c r="C49" s="379" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D49" s="8"/>
       <c r="E49" s="191"/>
@@ -16430,7 +16423,7 @@
       <c r="L49" s="156"/>
       <c r="M49" s="56"/>
       <c r="O49" s="233" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="P49" s="237"/>
       <c r="R49" s="312"/>
@@ -16438,7 +16431,7 @@
     <row r="50" spans="2:18" ht="16" thickBot="1">
       <c r="B50" s="37"/>
       <c r="C50" s="379" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D50" s="8"/>
       <c r="E50" s="171"/>
@@ -16451,7 +16444,7 @@
       <c r="L50" s="156"/>
       <c r="M50" s="56"/>
       <c r="O50" s="233" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="P50" s="237"/>
     </row>
@@ -16471,7 +16464,7 @@
       <c r="L51" s="156"/>
       <c r="M51" s="56"/>
       <c r="O51" s="233" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="P51" s="237"/>
     </row>
@@ -16523,7 +16516,7 @@
     <row r="54" spans="2:18">
       <c r="B54" s="37"/>
       <c r="C54" s="8" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D54" s="8"/>
       <c r="E54" s="59"/>
@@ -16556,7 +16549,7 @@
       <c r="L55" s="55"/>
       <c r="M55" s="56"/>
       <c r="O55" s="233" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="P55" s="237"/>
     </row>
@@ -16578,7 +16571,7 @@
       <c r="L56" s="55"/>
       <c r="M56" s="56"/>
       <c r="O56" s="233" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="P56" s="7"/>
     </row>
@@ -16598,7 +16591,7 @@
       <c r="L57" s="55"/>
       <c r="M57" s="56"/>
       <c r="O57" s="233" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="P57" s="7"/>
     </row>
@@ -16618,14 +16611,14 @@
       <c r="L58" s="55"/>
       <c r="M58" s="56"/>
       <c r="O58" s="233" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="P58" s="7"/>
     </row>
     <row r="59" spans="2:18" ht="16" thickBot="1">
       <c r="B59" s="37"/>
       <c r="C59" s="379" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D59" s="8"/>
       <c r="E59" s="171"/>
@@ -16638,7 +16631,7 @@
       <c r="L59" s="55"/>
       <c r="M59" s="56"/>
       <c r="O59" s="233" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="P59" s="7"/>
     </row>
@@ -16660,7 +16653,7 @@
     </row>
     <row r="61" spans="2:18">
       <c r="B61" s="302" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C61" s="53"/>
       <c r="D61" s="53"/>
@@ -16679,7 +16672,7 @@
     <row r="62" spans="2:18">
       <c r="B62" s="30"/>
       <c r="C62" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D62" s="8"/>
       <c r="E62" s="172">
@@ -16693,14 +16686,14 @@
       <c r="L62" s="8"/>
       <c r="M62" s="31"/>
       <c r="O62" s="233" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="P62" s="7"/>
     </row>
     <row r="63" spans="2:18">
       <c r="B63" s="30"/>
       <c r="C63" s="8" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D63" s="8"/>
       <c r="E63" s="172">
@@ -16714,7 +16707,7 @@
       <c r="L63" s="8"/>
       <c r="M63" s="31"/>
       <c r="O63" s="233" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="P63" s="7"/>
     </row>
@@ -16736,7 +16729,7 @@
     <row r="65" spans="2:16">
       <c r="B65" s="30"/>
       <c r="C65" s="8" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D65" s="8"/>
       <c r="E65" s="172">
@@ -16750,14 +16743,14 @@
       <c r="L65" s="8"/>
       <c r="M65" s="31"/>
       <c r="O65" s="233" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="P65" s="7"/>
     </row>
     <row r="66" spans="2:16">
       <c r="B66" s="30"/>
       <c r="C66" s="8" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D66" s="8"/>
       <c r="E66" s="172">
@@ -16771,7 +16764,7 @@
       <c r="L66" s="8"/>
       <c r="M66" s="31"/>
       <c r="O66" s="233" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="P66" s="7"/>
     </row>
@@ -16952,7 +16945,7 @@
   <sheetData>
     <row r="2" spans="2:67" ht="20">
       <c r="B2" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="3" spans="2:67" ht="15" customHeight="1">
@@ -23826,7 +23819,7 @@
     </row>
     <row r="5" spans="2:13">
       <c r="B5" s="403" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C5" s="404"/>
       <c r="D5" s="404"/>
@@ -23851,15 +23844,15 @@
     </row>
     <row r="7" spans="2:13">
       <c r="B7" s="324" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C7" s="325"/>
       <c r="D7" s="325"/>
       <c r="E7" s="326" t="s">
+        <v>565</v>
+      </c>
+      <c r="F7" s="322" t="s">
         <v>566</v>
-      </c>
-      <c r="F7" s="322" t="s">
-        <v>567</v>
       </c>
       <c r="G7" s="321"/>
       <c r="H7" s="322"/>
@@ -23868,7 +23861,7 @@
       <c r="K7" s="329"/>
       <c r="L7" s="333"/>
       <c r="M7" s="258" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="8" spans="2:13" ht="30">
@@ -23880,19 +23873,19 @@
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="347" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F8" s="8" t="s">
+        <v>542</v>
+      </c>
+      <c r="G8" s="8" t="s">
         <v>543</v>
       </c>
-      <c r="G8" s="8" t="s">
-        <v>544</v>
-      </c>
       <c r="H8" s="8" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I8" s="331" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="J8" s="334" t="s">
         <v>232</v>
@@ -23910,16 +23903,16 @@
       <c r="D9" s="74"/>
       <c r="E9" s="332"/>
       <c r="F9" s="323" t="s">
+        <v>544</v>
+      </c>
+      <c r="G9" s="323" t="s">
         <v>545</v>
       </c>
-      <c r="G9" s="323" t="s">
+      <c r="H9" s="323" t="s">
+        <v>562</v>
+      </c>
+      <c r="I9" s="11" t="s">
         <v>546</v>
-      </c>
-      <c r="H9" s="323" t="s">
-        <v>563</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>547</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="10"/>
@@ -23947,17 +23940,17 @@
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="345" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="F11" s="355"/>
       <c r="G11" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H11" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="I11" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="J11" s="366">
         <f>F11</f>
@@ -23969,7 +23962,7 @@
         <v>0</v>
       </c>
       <c r="M11" s="258" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="12" spans="2:13">
@@ -23979,15 +23972,15 @@
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="345" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F12" s="355"/>
       <c r="G12" s="355"/>
       <c r="H12" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="I12" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="J12" s="366"/>
       <c r="K12" s="360" t="e">
@@ -23999,7 +23992,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M12" s="258" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="13" spans="2:13">
@@ -24009,15 +24002,15 @@
       </c>
       <c r="D13" s="17"/>
       <c r="E13" s="345" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F13" s="355"/>
       <c r="G13" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H13" s="355"/>
       <c r="I13" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="J13" s="366"/>
       <c r="K13" s="360" t="e">
@@ -24029,7 +24022,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M13" s="258" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="14" spans="2:13">
@@ -24039,17 +24032,17 @@
       </c>
       <c r="D14" s="17"/>
       <c r="E14" s="345" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F14" s="355"/>
       <c r="G14" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H14" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="I14" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="J14" s="366">
         <f>F14</f>
@@ -24061,7 +24054,7 @@
         <v>0</v>
       </c>
       <c r="M14" s="258" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="15" spans="2:13">
@@ -24071,17 +24064,17 @@
       </c>
       <c r="D15" s="17"/>
       <c r="E15" s="345" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="F15" s="355"/>
       <c r="G15" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H15" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="I15" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="J15" s="366">
         <f>F15</f>
@@ -24093,7 +24086,7 @@
         <v>0</v>
       </c>
       <c r="M15" s="258" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="16" spans="2:13">
@@ -24103,17 +24096,17 @@
       </c>
       <c r="D16" s="17"/>
       <c r="E16" s="345" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="F16" s="355"/>
       <c r="G16" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H16" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="I16" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="J16" s="366">
         <f>F16</f>
@@ -24125,7 +24118,7 @@
         <v>0</v>
       </c>
       <c r="M16" s="258" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="17" spans="2:13">
@@ -24147,17 +24140,17 @@
       </c>
       <c r="D18" s="17"/>
       <c r="E18" s="345" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="F18" s="355"/>
       <c r="G18" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H18" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="I18" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="J18" s="366">
         <f>F18</f>
@@ -24169,7 +24162,7 @@
         <v>0</v>
       </c>
       <c r="M18" s="258" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="19" spans="2:13">
@@ -24179,17 +24172,17 @@
       </c>
       <c r="D19" s="17"/>
       <c r="E19" s="345" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F19" s="355"/>
       <c r="G19" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H19" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="I19" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="J19" s="366">
         <f>F19</f>
@@ -24201,7 +24194,7 @@
         <v>0</v>
       </c>
       <c r="M19" s="258" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="20" spans="2:13">
@@ -24211,17 +24204,17 @@
       </c>
       <c r="D20" s="17"/>
       <c r="E20" s="345" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F20" s="355"/>
       <c r="G20" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H20" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="I20" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="J20" s="366">
         <f>F20</f>
@@ -24233,7 +24226,7 @@
         <v>0</v>
       </c>
       <c r="M20" s="258" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="21" spans="2:13">
@@ -24272,17 +24265,17 @@
       </c>
       <c r="D23" s="17"/>
       <c r="E23" s="345" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F23" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="G23" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H23" s="355"/>
       <c r="I23" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="J23" s="366"/>
       <c r="K23" s="360" t="e">
@@ -24294,7 +24287,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M23" s="258" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="24" spans="2:13">
@@ -24304,17 +24297,17 @@
       </c>
       <c r="D24" s="17"/>
       <c r="E24" s="345" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F24" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="G24" s="355"/>
       <c r="H24" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="I24" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="J24" s="366"/>
       <c r="K24" s="360" t="e">
@@ -24326,7 +24319,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M24" s="258" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="25" spans="2:13">
@@ -24336,17 +24329,17 @@
       </c>
       <c r="D25" s="17"/>
       <c r="E25" s="345" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="F25" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="G25" s="355"/>
       <c r="H25" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="I25" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="J25" s="366"/>
       <c r="K25" s="360" t="e">
@@ -24358,7 +24351,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M25" s="258" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="26" spans="2:13">
@@ -24409,7 +24402,7 @@
         <v>0.05</v>
       </c>
       <c r="M28" s="258" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="29" spans="2:13">
@@ -24432,7 +24425,7 @@
         <v>0.12</v>
       </c>
       <c r="M29" s="258" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="30" spans="2:13">
@@ -24442,16 +24435,16 @@
       </c>
       <c r="D30" s="17"/>
       <c r="E30" s="345" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F30" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="G30" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H30" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="I30" s="355"/>
       <c r="J30" s="366">
@@ -24464,7 +24457,7 @@
         <v>0</v>
       </c>
       <c r="M30" s="258" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="31" spans="2:13">
@@ -24474,16 +24467,16 @@
       </c>
       <c r="D31" s="17"/>
       <c r="E31" s="345" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="F31" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="G31" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H31" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="I31" s="355"/>
       <c r="J31" s="366">
@@ -24496,7 +24489,7 @@
         <v>0</v>
       </c>
       <c r="M31" s="258" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="32" spans="2:13">
@@ -24506,16 +24499,16 @@
       </c>
       <c r="D32" s="17"/>
       <c r="E32" s="345" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F32" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="G32" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H32" s="355" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="I32" s="355"/>
       <c r="J32" s="366">
@@ -24528,7 +24521,7 @@
         <v>0</v>
       </c>
       <c r="M32" s="258" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="33" spans="2:12" ht="16" thickBot="1">

</xml_diff>